<commit_message>
changed chart data and styles
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03636123882d8546/Documents/Udacity/stackoverflow_research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SCO2186893\Documents\Udacity\stackoverflow_research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="8_{F5A8D57F-AE3F-4F31-8803-AE207806FF74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{43D36441-3E85-495D-8B4F-EC2DF8952D47}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{6DA26B7D-D8D4-413E-993A-55622C42E696}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>Master's Degree</t>
   </si>
@@ -165,13 +164,22 @@
   </si>
   <si>
     <t>Job Role</t>
+  </si>
+  <si>
+    <t>Mixed Data Scientist Role</t>
+  </si>
+  <si>
+    <t>Pure Data Scientist Role</t>
+  </si>
+  <si>
+    <t>Non Data Scientist Role</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +192,13 @@
       <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -206,9 +221,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -261,11 +278,26 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Data Scientist Highest Education Level</a:t>
+              <a:t>Maximum</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Education Levels</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -305,6 +337,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mixed Data Scientist Role</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -348,29 +391,195 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>12.1</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35.6</c:v>
+                  <c:v>34.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35</c:v>
+                  <c:v>35.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6</c:v>
+                  <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.5</c:v>
+                  <c:v>6.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.2</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CEF4-4766-A7AA-28D362B6D008}"/>
+              <c16:uniqueId val="{00000000-24BD-43CB-BD19-6C6E82E90F4A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pure Data Scientist Role</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Doctoral Degree</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Master's Degree</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Bachelor's Degree</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Associate Degree</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Some College (No Degree)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Secondary School</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-24BD-43CB-BD19-6C6E82E90F4A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Non Data Scientist Role</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Doctoral Degree</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Master's Degree</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Bachelor's Degree</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Associate Degree</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Some College (No Degree)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Secondary School</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-24BD-43CB-BD19-6C6E82E90F4A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -384,11 +593,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="681864688"/>
-        <c:axId val="681867640"/>
+        <c:axId val="190804176"/>
+        <c:axId val="190806800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="681864688"/>
+        <c:axId val="190804176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -431,7 +640,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="681867640"/>
+        <c:crossAx val="190806800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -439,7 +648,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="681867640"/>
+        <c:axId val="190806800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -459,6 +668,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percentage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -490,7 +755,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="681864688"/>
+        <c:crossAx val="190804176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -502,6 +767,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -574,16 +871,17 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Data</a:t>
+              <a:t>Undergraduate</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Scientist Undergrad Major</a:t>
+              <a:t> Majors</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -623,6 +921,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mixed Data Scientist Role</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -684,28 +993,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>47.5</c:v>
+                  <c:v>49.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.6</c:v>
+                  <c:v>9.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.4</c:v>
+                  <c:v>10.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.6</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.6</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.9</c:v>
@@ -717,14 +1026,252 @@
                   <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.3</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-518E-4095-9A02-CB0D6EEDB8E4}"/>
+              <c16:uniqueId val="{00000000-CA74-4967-894B-FA867F1EDB65}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pure Data Scientist Role</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$19:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>CS, CE, or SE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Math or statistics </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Natural sciences </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Other engineering discipline </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Info systems, IT, or sysadmin</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Social sciences</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Business</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Humanities</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Web dev/design</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Health sciences</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Fine/Performing arts </c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Undeclared</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$19:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>28.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CA74-4967-894B-FA867F1EDB65}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Non Data Scientist Role</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$19:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>CS, CE, or SE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Math or statistics </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Natural sciences </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Other engineering discipline </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Info systems, IT, or sysadmin</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Social sciences</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Business</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Humanities</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Web dev/design</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Health sciences</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Fine/Performing arts </c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Undeclared</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$19:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>56.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-CA74-4967-894B-FA867F1EDB65}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -737,11 +1284,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="751205480"/>
-        <c:axId val="751200232"/>
+        <c:axId val="290586336"/>
+        <c:axId val="290586664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="751205480"/>
+        <c:axId val="290586336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -784,7 +1331,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="751200232"/>
+        <c:crossAx val="290586664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -792,7 +1339,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="751200232"/>
+        <c:axId val="290586664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -843,7 +1390,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="751205480"/>
+        <c:crossAx val="290586336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -855,6 +1402,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -913,7 +1492,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -927,11 +1506,24 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Job Roles For Data Scientists vs. Non-Data Scientists</a:t>
+              <a:t>Other Data</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Scientist Job Roles</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.47923287739337406"/>
+          <c:y val="1.6922258655169005E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -945,7 +1537,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -983,42 +1575,13 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -1178,221 +1741,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-34F2-4D46-8815-4A3A21361C17}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$37</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Non-DS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$38:$A$60</c:f>
-              <c:strCache>
-                <c:ptCount val="23"/>
-                <c:pt idx="0">
-                  <c:v>Developer, back-end                          </c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Developer, full-stack                        </c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Data or business analyst                     </c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Academic researcher                          </c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Engineer, data                               </c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Scientist                                    </c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Student                                      </c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Developer, front-end                         </c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Database administrator                       </c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Developer, desktop or enterprise applications</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>System administrator                         </c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Developer, mobile                            </c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Designer                                     </c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>DevOps specialist                            </c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Educator                                     </c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Developer, embedded applications or devices  </c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Developer, QA or test                        </c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Product manager                              </c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Developer, game or graphics                  </c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Engineering manager                          </c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Engineer, site reliability                   </c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Senior executive/VP                          </c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Marketing or sales professional              </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$38:$C$60</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
-                <c:pt idx="0">
-                  <c:v>16.899999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>17.899999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>11.4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6.2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.6</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.7</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.9</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2.6</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.6</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.8</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.7</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-34F2-4D46-8815-4A3A21361C17}"/>
+              <c16:uniqueId val="{00000000-67E7-44F3-B0B7-90A210E216CC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1404,13 +1753,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="115"/>
-        <c:overlap val="-20"/>
-        <c:axId val="751204168"/>
-        <c:axId val="751205152"/>
+        <c:gapWidth val="182"/>
+        <c:axId val="622205856"/>
+        <c:axId val="622206184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="751204168"/>
+        <c:axId val="622205856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1422,7 +1770,7 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -1453,7 +1801,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="751205152"/>
+        <c:crossAx val="622206184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1461,7 +1809,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="751205152"/>
+        <c:axId val="622206184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1512,7 +1860,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="751204168"/>
+        <c:crossAx val="622205856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1524,37 +1872,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2721,7 +3038,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="341">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2732,7 +3049,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -2745,7 +3062,7 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
@@ -2762,7 +3079,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2778,7 +3095,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -2822,20 +3139,20 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -2844,13 +3161,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="34925" cap="rnd">
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2862,10 +3179,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -2874,17 +3191,16 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -2926,22 +3242,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2988,8 +3305,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -3040,8 +3363,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3079,20 +3402,20 @@
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -3105,17 +3428,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -3147,7 +3459,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -3156,13 +3468,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -3183,19 +3496,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3216,8 +3530,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3227,25 +3547,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>14287</xdr:colOff>
+      <xdr:colOff>69055</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:rowOff>35717</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>319087</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>42862</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CF713D7-4787-47DB-ABE1-C32FB2F17508}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3262,26 +3576,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>595311</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>40480</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>121443</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>47624</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>109538</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CD11D07-00F3-4B48-9930-A04313431C62}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3298,26 +3606,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>585786</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>16668</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>7142</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>623888</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1080DE74-A771-408A-9018-55EE4BE71883}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3631,217 +3933,302 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C6E585-71A8-43E9-8419-D9AD87F52C8B}">
-  <dimension ref="A2:C60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="71.7109375" customWidth="1"/>
+    <col min="1" max="1" width="71.73046875" customWidth="1"/>
+    <col min="2" max="2" width="8.3984375" customWidth="1"/>
+    <col min="3" max="3" width="7.73046875" customWidth="1"/>
+    <col min="4" max="4" width="9.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>12.1</v>
+        <v>11.5</v>
+      </c>
+      <c r="C2">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3">
-        <v>35.6</v>
+        <v>34.5</v>
+      </c>
+      <c r="C3">
+        <v>47.9</v>
+      </c>
+      <c r="D3">
+        <v>22.1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>35</v>
+        <v>35.700000000000003</v>
+      </c>
+      <c r="C4">
+        <v>27</v>
+      </c>
+      <c r="D4">
+        <v>47.2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1.6</v>
+        <v>1.7</v>
+      </c>
+      <c r="C5">
+        <v>0.6</v>
+      </c>
+      <c r="D5">
+        <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
-        <v>6.5</v>
+        <v>6.9</v>
+      </c>
+      <c r="C6">
+        <v>1.9</v>
+      </c>
+      <c r="D6">
+        <v>12.3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>5.2</v>
+        <v>5.5</v>
+      </c>
+      <c r="C7">
+        <v>1.7</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>22.1</v>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <v>49.2</v>
+      </c>
+      <c r="C19">
+        <v>28.1</v>
+      </c>
+      <c r="D19">
+        <v>56.2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>47.2</v>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>9.9</v>
+      </c>
+      <c r="C20">
+        <v>30.4</v>
+      </c>
+      <c r="D20">
+        <v>2.7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12">
-        <v>3.5</v>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>10.1</v>
+      </c>
+      <c r="C21">
+        <v>13.1</v>
+      </c>
+      <c r="D21">
+        <v>3.2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13">
-        <v>12.3</v>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <v>8.5</v>
+      </c>
+      <c r="C22">
+        <v>10.5</v>
+      </c>
+      <c r="D22">
+        <v>7.1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19">
-        <v>47.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20">
-        <v>11.6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21">
-        <v>10.4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22">
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B23">
         <v>3.6</v>
       </c>
+      <c r="C23">
+        <v>3.2</v>
+      </c>
+      <c r="D23">
+        <v>6.4</v>
+      </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B24">
-        <v>2.6</v>
+        <v>2.5</v>
+      </c>
+      <c r="C24">
+        <v>4.2</v>
+      </c>
+      <c r="D24">
+        <v>1.5</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B25">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
+      </c>
+      <c r="C25">
+        <v>1.7</v>
+      </c>
+      <c r="D25">
+        <v>2.1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B26">
-        <v>1.3</v>
+        <v>1.2</v>
+      </c>
+      <c r="C26">
+        <v>1.7</v>
+      </c>
+      <c r="D26">
+        <v>1.8</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B27">
         <v>0.9</v>
       </c>
+      <c r="C27">
+        <v>0.4</v>
+      </c>
+      <c r="D27">
+        <v>4.3</v>
+      </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B28">
         <v>0.6</v>
       </c>
+      <c r="C28">
+        <v>0.6</v>
+      </c>
+      <c r="D28">
+        <v>0.3</v>
+      </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B29">
         <v>0.6</v>
       </c>
+      <c r="C29">
+        <v>0.2</v>
+      </c>
+      <c r="D29">
+        <v>1.5</v>
+      </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B30">
-        <v>0.3</v>
+        <v>0.4</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -3852,7 +4239,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>18</v>
       </c>
@@ -3863,7 +4250,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -3874,7 +4261,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>20</v>
       </c>
@@ -3885,7 +4272,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -3896,7 +4283,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -3907,7 +4294,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>23</v>
       </c>
@@ -3918,7 +4305,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>24</v>
       </c>
@@ -3929,7 +4316,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>25</v>
       </c>
@@ -3940,7 +4327,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -3951,7 +4338,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>27</v>
       </c>
@@ -3962,7 +4349,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>28</v>
       </c>
@@ -3973,7 +4360,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>29</v>
       </c>
@@ -3984,7 +4371,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>30</v>
       </c>
@@ -3995,7 +4382,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -4006,7 +4393,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>32</v>
       </c>
@@ -4017,7 +4404,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>33</v>
       </c>
@@ -4028,7 +4415,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>34</v>
       </c>
@@ -4039,7 +4426,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>35</v>
       </c>
@@ -4050,7 +4437,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>36</v>
       </c>
@@ -4061,7 +4448,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>37</v>
       </c>
@@ -4072,7 +4459,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>38</v>
       </c>
@@ -4083,7 +4470,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>39</v>
       </c>
@@ -4094,7 +4481,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>40</v>
       </c>
@@ -4107,7 +4494,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
broke out language/database charts
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SCO2186893\Documents\Udacity\stackoverflow_research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\OneDrive\Documents\Udacity\stackoverflow_research\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="57" documentId="114_{E02A7B06-5038-4768-895C-47E222B8DDA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{87C79EB0-1DC0-4E00-8F34-CCF8F155E71A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="74">
   <si>
     <t>Master's Degree</t>
   </si>
@@ -252,11 +245,14 @@
   <si>
     <t>Couchbase</t>
   </si>
+  <si>
+    <t>Go</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -375,7 +371,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -772,7 +767,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -847,7 +841,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -959,7 +952,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1482,7 +1474,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2022,12 +2013,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Top 10 Programming Languages Used vs Desired</a:t>
+              <a:t>Programming Languages</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Used</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> In 2019</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2061,7 +2059,7 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="col"/>
+        <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -2167,114 +2165,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5078-4D14-8F20-9EC9124812BF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$71</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Desired For 2020</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$72:$A$81</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Python</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>SQL</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>R</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Bash/Shell/PowerShell</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>HTML/CSS</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>JavaScript</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Java </c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>C++</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>C</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Scala</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$72:$C$81</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5078-4D14-8F20-9EC9124812BF}"/>
+              <c16:uniqueId val="{00000000-A376-4365-94A7-3FBC30435074}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2286,18 +2177,17 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="36665200"/>
-        <c:axId val="36660608"/>
+        <c:gapWidth val="182"/>
+        <c:axId val="467137912"/>
+        <c:axId val="467139224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="36665200"/>
+        <c:axId val="467137912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2335,7 +2225,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36660608"/>
+        <c:crossAx val="467139224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2343,12 +2233,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36660608"/>
+        <c:axId val="467139224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2394,7 +2284,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36665200"/>
+        <c:crossAx val="467137912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2406,38 +2296,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2510,12 +2368,352 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Databases Used vs Desired</a:t>
+              <a:t>Programming Languages Wanting</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> To Be Used In 2020</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$88:$A$97</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Python</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>R</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SQL</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Bash/Shell/PowerShell</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scala</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>C++</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>JavaScript</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>HTML/CSS</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Other(s)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Go</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$88:$B$97</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1024-46AC-96CD-F2C5335C0ABF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="223928848"/>
+        <c:axId val="223926880"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="223928848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="223926880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="223926880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="223928848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Databases Used In 2019</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2555,17 +2753,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$93</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Used In 2019</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2578,7 +2765,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$94:$A$107</c:f>
+              <c:f>Sheet1!$A$107:$A$120</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -2628,7 +2815,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$94:$B$107</c:f>
+              <c:f>Sheet1!$B$107:$B$120</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2679,138 +2866,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-35C8-4F59-96D2-6F280D62676B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$93</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Desired For 2020</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$94:$A$107</c:f>
-              <c:strCache>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>PostgreSQL</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>MySQL</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>MS SQL Server</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>SQLite</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>MongoDB</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Elasticsearch</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Oracle</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Other(s)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Redis</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Cassandra</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>DynamoDB</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>MariaDB</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Firebase</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Couchbase</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$94:$C$107</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>19.100000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13.1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>13.9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.7</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.9</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-35C8-4F59-96D2-6F280D62676B}"/>
+              <c16:uniqueId val="{00000000-36BC-4123-B634-7518CBABF608}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2824,11 +2880,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="302930176"/>
-        <c:axId val="302928208"/>
+        <c:axId val="662932208"/>
+        <c:axId val="662932536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="302930176"/>
+        <c:axId val="662932208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2871,7 +2927,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302928208"/>
+        <c:crossAx val="662932536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2879,7 +2935,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="302928208"/>
+        <c:axId val="662932536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2930,7 +2986,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302930176"/>
+        <c:crossAx val="662932208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2942,9 +2998,88 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Databases Wanting</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> To Be Used In 2020</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2958,7 +3093,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2973,7 +3108,262 @@
           <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
-    </c:legend>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$122:$A$135</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>PostgreSQL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MongoDB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MySQL</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MS SQL Server</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Elasticsearch</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>SQLite</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Redis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Cassandra</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Other(s)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>DynamoDB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Oracle</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>MariaDB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Firebase</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Couchbase</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$122:$B$135</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>19.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1923-48D4-9AD3-FF9B111C7678}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="667604648"/>
+        <c:axId val="667605304"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="667604648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="667605304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="667605304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="667604648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3211,6 +3601,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4725,7 +5195,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4929,6 +5399,1016 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
@@ -5227,7 +6707,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5747,7 +7227,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5777,7 +7263,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5807,7 +7299,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5824,20 +7322,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>645318</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>35717</xdr:rowOff>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>595313</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1A5D567-403C-4224-8068-DE9BA5831372}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5855,19 +7359,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>7142</xdr:colOff>
-      <xdr:row>92</xdr:row>
-      <xdr:rowOff>26192</xdr:rowOff>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>14287</xdr:colOff>
-      <xdr:row>113</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98706737-B4CA-4A62-AE0C-26958FFBCD20}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5877,6 +7387,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CA5A009-9937-4BC9-BA40-38DE1C24886B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58B2FBBD-20A7-4F27-98B1-45914BA51EFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6181,22 +7763,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D107"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="R105" sqref="R105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="71.73046875" customWidth="1"/>
-    <col min="2" max="2" width="8.3984375" customWidth="1"/>
-    <col min="3" max="3" width="7.73046875" customWidth="1"/>
-    <col min="4" max="4" width="9.19921875" customWidth="1"/>
+    <col min="1" max="1" width="71.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>44</v>
       </c>
@@ -6207,7 +7789,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -6221,7 +7803,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -6235,7 +7817,7 @@
         <v>22.1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -6249,7 +7831,7 @@
         <v>47.2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -6263,7 +7845,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -6277,7 +7859,7 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -6291,7 +7873,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>44</v>
       </c>
@@ -6302,7 +7884,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
@@ -6316,7 +7898,7 @@
         <v>56.2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -6330,7 +7912,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -6344,7 +7926,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>9</v>
       </c>
@@ -6358,7 +7940,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>10</v>
       </c>
@@ -6372,7 +7954,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
@@ -6386,7 +7968,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>13</v>
       </c>
@@ -6400,7 +7982,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>14</v>
       </c>
@@ -6414,7 +7996,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>15</v>
       </c>
@@ -6428,7 +8010,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>16</v>
       </c>
@@ -6442,7 +8024,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>17</v>
       </c>
@@ -6456,7 +8038,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>6</v>
       </c>
@@ -6470,13 +8052,13 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -6487,7 +8069,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>18</v>
       </c>
@@ -6498,7 +8080,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -6509,7 +8091,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>20</v>
       </c>
@@ -6520,7 +8102,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -6531,7 +8113,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -6542,7 +8124,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>23</v>
       </c>
@@ -6553,7 +8135,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>24</v>
       </c>
@@ -6564,7 +8146,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>25</v>
       </c>
@@ -6575,7 +8157,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -6586,7 +8168,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>27</v>
       </c>
@@ -6597,7 +8179,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>28</v>
       </c>
@@ -6608,7 +8190,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>29</v>
       </c>
@@ -6619,7 +8201,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>30</v>
       </c>
@@ -6630,7 +8212,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -6641,7 +8223,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>32</v>
       </c>
@@ -6652,7 +8234,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>33</v>
       </c>
@@ -6663,7 +8245,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>34</v>
       </c>
@@ -6674,7 +8256,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>35</v>
       </c>
@@ -6685,7 +8267,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>36</v>
       </c>
@@ -6696,7 +8278,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>37</v>
       </c>
@@ -6707,7 +8289,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>38</v>
       </c>
@@ -6718,7 +8300,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>39</v>
       </c>
@@ -6729,7 +8311,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>40</v>
       </c>
@@ -6740,7 +8322,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>57</v>
       </c>
@@ -6748,7 +8330,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>47</v>
       </c>
@@ -6759,7 +8341,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>48</v>
       </c>
@@ -6770,7 +8352,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>54</v>
       </c>
@@ -6781,7 +8363,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>51</v>
       </c>
@@ -6792,7 +8374,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>50</v>
       </c>
@@ -6803,7 +8385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>49</v>
       </c>
@@ -6814,7 +8396,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>52</v>
       </c>
@@ -6825,7 +8407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>53</v>
       </c>
@@ -6836,7 +8418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>55</v>
       </c>
@@ -6847,7 +8429,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>56</v>
       </c>
@@ -6858,165 +8440,312 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B93" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>47</v>
+      </c>
+      <c r="B88">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>54</v>
+      </c>
+      <c r="B89">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>48</v>
+      </c>
+      <c r="B90">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>51</v>
+      </c>
+      <c r="B91">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>56</v>
+      </c>
+      <c r="B92">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>53</v>
+      </c>
+      <c r="B93">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>49</v>
+      </c>
+      <c r="B94">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>50</v>
+      </c>
+      <c r="B95">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>66</v>
+      </c>
+      <c r="B96">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>73</v>
+      </c>
+      <c r="B97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
         <v>57</v>
       </c>
-      <c r="C93" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A94" t="s">
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>59</v>
       </c>
-      <c r="B94">
+      <c r="B107">
         <v>18.600000000000001</v>
       </c>
-      <c r="C94">
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>60</v>
+      </c>
+      <c r="B108">
+        <v>17.7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>61</v>
+      </c>
+      <c r="B109">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>62</v>
+      </c>
+      <c r="B110">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>63</v>
+      </c>
+      <c r="B111">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>64</v>
+      </c>
+      <c r="B112">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>65</v>
+      </c>
+      <c r="B113">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>66</v>
+      </c>
+      <c r="B114">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>67</v>
+      </c>
+      <c r="B115">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>68</v>
+      </c>
+      <c r="B116">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>69</v>
+      </c>
+      <c r="B117">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>70</v>
+      </c>
+      <c r="B118">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>71</v>
+      </c>
+      <c r="B119">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>72</v>
+      </c>
+      <c r="B120">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>59</v>
+      </c>
+      <c r="B122">
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A95" t="s">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>63</v>
+      </c>
+      <c r="B123">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>60</v>
       </c>
-      <c r="B95">
-        <v>17.7</v>
-      </c>
-      <c r="C95">
+      <c r="B124">
         <v>13.1</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A96" t="s">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>61</v>
       </c>
-      <c r="B96">
-        <v>12.4</v>
-      </c>
-      <c r="C96">
+      <c r="B125">
         <v>13.1</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A97" t="s">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>64</v>
+      </c>
+      <c r="B126">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>62</v>
       </c>
-      <c r="B97">
-        <v>10.5</v>
-      </c>
-      <c r="C97">
+      <c r="B127">
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A98" t="s">
-        <v>63</v>
-      </c>
-      <c r="B98">
-        <v>10.4</v>
-      </c>
-      <c r="C98">
-        <v>13.9</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A99" t="s">
-        <v>64</v>
-      </c>
-      <c r="B99">
-        <v>7</v>
-      </c>
-      <c r="C99">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A100" t="s">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>67</v>
+      </c>
+      <c r="B128">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>68</v>
+      </c>
+      <c r="B129">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>66</v>
+      </c>
+      <c r="B130">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>69</v>
+      </c>
+      <c r="B131">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>65</v>
       </c>
-      <c r="B100">
-        <v>6.2</v>
-      </c>
-      <c r="C100">
+      <c r="B132">
         <v>2.5</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A101" t="s">
-        <v>66</v>
-      </c>
-      <c r="B101">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="C101">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A102" t="s">
-        <v>67</v>
-      </c>
-      <c r="B102">
-        <v>3.9</v>
-      </c>
-      <c r="C102">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A103" t="s">
-        <v>68</v>
-      </c>
-      <c r="B103">
-        <v>2.9</v>
-      </c>
-      <c r="C103">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A104" t="s">
-        <v>69</v>
-      </c>
-      <c r="B104">
-        <v>2.8</v>
-      </c>
-      <c r="C104">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A105" t="s">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>70</v>
       </c>
-      <c r="B105">
-        <v>1.7</v>
-      </c>
-      <c r="C105">
+      <c r="B133">
         <v>2.4</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A106" t="s">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>71</v>
       </c>
-      <c r="B106">
-        <v>0.8</v>
-      </c>
-      <c r="C106">
+      <c r="B134">
         <v>1.9</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A107" t="s">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>72</v>
       </c>
-      <c r="B107">
-        <v>0.4</v>
-      </c>
-      <c r="C107">
+      <c r="B135">
         <v>0.9</v>
       </c>
     </row>

</xml_diff>